<commit_message>
Record disappears when pressing the process button, for validations between dates per month
</commit_message>
<xml_diff>
--- a/storage/app/public/users/jose.jdgo97/COACTIVO.xlsx
+++ b/storage/app/public/users/jose.jdgo97/COACTIVO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\www\LARAVEL\versiones cam\multimedia_cam4\public\storage\users\jose.jdgo97\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2EDC57-07A3-4947-9438-00BA07AA5265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748491B3-42B8-4497-8097-B48E47370968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39780,7 +39780,7 @@
         <v>15</v>
       </c>
       <c r="O9" s="15">
-        <v>45724</v>
+        <v>45715</v>
       </c>
       <c r="P9" s="16">
         <v>0.64959490740740744</v>

</xml_diff>